<commit_message>
26 Aug 2025 Regular No Supply
</commit_message>
<xml_diff>
--- a/Result_Regular.xlsx
+++ b/Result_Regular.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="454">
   <si>
     <t>Sl.No</t>
   </si>
@@ -1355,6 +1355,30 @@
   <si>
     <t>C SRINITYA</t>
   </si>
+  <si>
+    <t>2401100CSE0079</t>
+  </si>
+  <si>
+    <t>GANTA KOUSHIK REDDY</t>
+  </si>
+  <si>
+    <t>2401100CSE0118</t>
+  </si>
+  <si>
+    <t>BACHU GNANA PRASUNA</t>
+  </si>
+  <si>
+    <t>24011CSEAI0026</t>
+  </si>
+  <si>
+    <t>KANDUKOORI ANUDEEP</t>
+  </si>
+  <si>
+    <t>24011CSEAI0033</t>
+  </si>
+  <si>
+    <t>MAHAJAN SANKEERTHANA</t>
+  </si>
 </sst>
 </file>
 
@@ -20792,1208 +20816,1504 @@
       </c>
     </row>
     <row r="152" ht="18.0" customHeight="1">
-      <c r="A152" s="35">
+      <c r="A152" s="34">
         <v>150.0</v>
       </c>
-      <c r="B152" s="36" t="s">
+      <c r="B152" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="C152" s="36" t="s">
+      <c r="C152" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="D152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E152" s="37" t="s">
+      <c r="D152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E152" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F152" s="37">
+      <c r="F152" s="27">
         <v>4.0</v>
       </c>
-      <c r="G152" s="37" t="s">
+      <c r="G152" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I152" s="37" t="s">
+      <c r="H152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I152" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J152" s="38">
+      <c r="J152" s="28">
         <v>3.0</v>
       </c>
-      <c r="K152" s="38" t="s">
+      <c r="K152" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M152" s="37" t="s">
+      <c r="L152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M152" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="N152" s="37">
+      <c r="N152" s="27">
         <v>4.0</v>
       </c>
-      <c r="O152" s="37" t="s">
+      <c r="O152" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P152" s="39"/>
-      <c r="Q152" s="39"/>
-      <c r="R152" s="39"/>
-      <c r="S152" s="39"/>
-      <c r="T152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="U152" s="37" t="s">
+      <c r="P152" s="21"/>
+      <c r="Q152" s="21"/>
+      <c r="R152" s="21"/>
+      <c r="S152" s="21"/>
+      <c r="T152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U152" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="V152" s="37">
+      <c r="V152" s="27">
         <v>3.0</v>
       </c>
-      <c r="W152" s="37" t="s">
+      <c r="W152" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="X152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y152" s="37" t="s">
+      <c r="X152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y152" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Z152" s="37">
+      <c r="Z152" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA152" s="37" t="s">
+      <c r="AA152" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC152" s="37" t="s">
+      <c r="AB152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC152" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AD152" s="37">
+      <c r="AD152" s="27">
         <v>2.0</v>
       </c>
-      <c r="AE152" s="37" t="s">
+      <c r="AE152" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AF152" s="39"/>
-      <c r="AG152" s="39"/>
-      <c r="AH152" s="39"/>
-      <c r="AI152" s="39"/>
-      <c r="AJ152" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK152" s="37" t="s">
+      <c r="AF152" s="21"/>
+      <c r="AG152" s="21"/>
+      <c r="AH152" s="21"/>
+      <c r="AI152" s="21"/>
+      <c r="AJ152" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK152" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AL152" s="37">
+      <c r="AL152" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM152" s="37" t="s">
+      <c r="AM152" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN152" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO152" s="38" t="s">
+      <c r="AN152" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO152" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AP152" s="38">
+      <c r="AP152" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ152" s="38" t="s">
+      <c r="AQ152" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR152" s="39"/>
-      <c r="AS152" s="39"/>
-      <c r="AT152" s="39"/>
-      <c r="AU152" s="39"/>
-      <c r="AV152" s="40">
+      <c r="AR152" s="21"/>
+      <c r="AS152" s="21"/>
+      <c r="AT152" s="21"/>
+      <c r="AU152" s="21"/>
+      <c r="AV152" s="30">
         <v>9.14</v>
       </c>
-      <c r="AW152" s="40">
+      <c r="AW152" s="30">
         <v>9.48</v>
       </c>
     </row>
     <row r="153" ht="18.0" customHeight="1">
-      <c r="A153" s="35">
+      <c r="A153" s="34">
         <v>151.0</v>
       </c>
-      <c r="B153" s="36" t="s">
+      <c r="B153" s="26" t="s">
         <v>432</v>
       </c>
-      <c r="C153" s="36" t="s">
+      <c r="C153" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="D153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E153" s="37" t="s">
+      <c r="D153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F153" s="37">
+      <c r="F153" s="27">
         <v>4.0</v>
       </c>
-      <c r="G153" s="37" t="s">
+      <c r="G153" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I153" s="37" t="s">
+      <c r="H153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I153" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J153" s="38">
+      <c r="J153" s="28">
         <v>3.0</v>
       </c>
-      <c r="K153" s="38" t="s">
+      <c r="K153" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M153" s="37" t="s">
+      <c r="L153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M153" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="N153" s="37">
+      <c r="N153" s="27">
         <v>4.0</v>
       </c>
-      <c r="O153" s="37" t="s">
+      <c r="O153" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P153" s="39"/>
-      <c r="Q153" s="39"/>
-      <c r="R153" s="39"/>
-      <c r="S153" s="39"/>
-      <c r="T153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="U153" s="37" t="s">
+      <c r="P153" s="21"/>
+      <c r="Q153" s="21"/>
+      <c r="R153" s="21"/>
+      <c r="S153" s="21"/>
+      <c r="T153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U153" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="V153" s="37">
+      <c r="V153" s="27">
         <v>3.0</v>
       </c>
-      <c r="W153" s="37" t="s">
+      <c r="W153" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="X153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y153" s="37" t="s">
+      <c r="X153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y153" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Z153" s="37">
+      <c r="Z153" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA153" s="37" t="s">
+      <c r="AA153" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC153" s="37" t="s">
+      <c r="AB153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC153" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="AD153" s="37">
+      <c r="AD153" s="27">
         <v>2.0</v>
       </c>
-      <c r="AE153" s="37" t="s">
+      <c r="AE153" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AF153" s="39"/>
-      <c r="AG153" s="39"/>
-      <c r="AH153" s="39"/>
-      <c r="AI153" s="39"/>
-      <c r="AJ153" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK153" s="37" t="s">
+      <c r="AF153" s="21"/>
+      <c r="AG153" s="21"/>
+      <c r="AH153" s="21"/>
+      <c r="AI153" s="21"/>
+      <c r="AJ153" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK153" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL153" s="37">
+      <c r="AL153" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM153" s="37" t="s">
+      <c r="AM153" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN153" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO153" s="38" t="s">
+      <c r="AN153" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO153" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AP153" s="38">
+      <c r="AP153" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ153" s="38" t="s">
+      <c r="AQ153" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR153" s="39"/>
-      <c r="AS153" s="39"/>
-      <c r="AT153" s="39"/>
-      <c r="AU153" s="39"/>
-      <c r="AV153" s="40">
+      <c r="AR153" s="21"/>
+      <c r="AS153" s="21"/>
+      <c r="AT153" s="21"/>
+      <c r="AU153" s="21"/>
+      <c r="AV153" s="30">
         <v>7.46</v>
       </c>
-      <c r="AW153" s="40">
+      <c r="AW153" s="30">
         <v>7.72</v>
       </c>
     </row>
     <row r="154" ht="18.0" customHeight="1">
-      <c r="A154" s="35">
+      <c r="A154" s="34">
         <v>152.0</v>
       </c>
-      <c r="B154" s="36" t="s">
+      <c r="B154" s="26" t="s">
         <v>434</v>
       </c>
-      <c r="C154" s="36" t="s">
+      <c r="C154" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="D154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E154" s="37" t="s">
+      <c r="D154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E154" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F154" s="37">
+      <c r="F154" s="27">
         <v>4.0</v>
       </c>
-      <c r="G154" s="37" t="s">
+      <c r="G154" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I154" s="37" t="s">
+      <c r="H154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I154" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J154" s="38">
+      <c r="J154" s="28">
         <v>3.0</v>
       </c>
-      <c r="K154" s="38" t="s">
+      <c r="K154" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M154" s="37" t="s">
+      <c r="L154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M154" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="N154" s="37">
+      <c r="N154" s="27">
         <v>4.0</v>
       </c>
-      <c r="O154" s="37" t="s">
+      <c r="O154" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P154" s="39"/>
-      <c r="Q154" s="39"/>
-      <c r="R154" s="39"/>
-      <c r="S154" s="39"/>
-      <c r="T154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="U154" s="37" t="s">
+      <c r="P154" s="21"/>
+      <c r="Q154" s="21"/>
+      <c r="R154" s="21"/>
+      <c r="S154" s="21"/>
+      <c r="T154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="U154" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="V154" s="37">
+      <c r="V154" s="27">
         <v>3.0</v>
       </c>
-      <c r="W154" s="37" t="s">
+      <c r="W154" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="X154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y154" s="37" t="s">
+      <c r="X154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y154" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Z154" s="37">
+      <c r="Z154" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA154" s="37" t="s">
+      <c r="AA154" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC154" s="37" t="s">
+      <c r="AB154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC154" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AD154" s="37">
+      <c r="AD154" s="27">
         <v>2.0</v>
       </c>
-      <c r="AE154" s="37" t="s">
+      <c r="AE154" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="AF154" s="39"/>
-      <c r="AG154" s="39"/>
-      <c r="AH154" s="39"/>
-      <c r="AI154" s="39"/>
-      <c r="AJ154" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK154" s="37" t="s">
+      <c r="AF154" s="21"/>
+      <c r="AG154" s="21"/>
+      <c r="AH154" s="21"/>
+      <c r="AI154" s="21"/>
+      <c r="AJ154" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK154" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL154" s="37">
+      <c r="AL154" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM154" s="37" t="s">
+      <c r="AM154" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN154" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO154" s="38" t="s">
+      <c r="AN154" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO154" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AP154" s="38">
+      <c r="AP154" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ154" s="38" t="s">
+      <c r="AQ154" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR154" s="39"/>
-      <c r="AS154" s="39"/>
-      <c r="AT154" s="39"/>
-      <c r="AU154" s="39"/>
-      <c r="AV154" s="40">
+      <c r="AR154" s="21"/>
+      <c r="AS154" s="21"/>
+      <c r="AT154" s="21"/>
+      <c r="AU154" s="21"/>
+      <c r="AV154" s="30">
         <v>7.55</v>
       </c>
-      <c r="AW154" s="40">
+      <c r="AW154" s="30">
         <v>7.79</v>
       </c>
     </row>
     <row r="155" ht="18.0" customHeight="1">
-      <c r="A155" s="35">
+      <c r="A155" s="34">
         <v>153.0</v>
       </c>
-      <c r="B155" s="36" t="s">
+      <c r="B155" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="C155" s="36" t="s">
+      <c r="C155" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="D155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E155" s="37" t="s">
+      <c r="D155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E155" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F155" s="37">
+      <c r="F155" s="27">
         <v>4.0</v>
       </c>
-      <c r="G155" s="37" t="s">
+      <c r="G155" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I155" s="37" t="s">
+      <c r="H155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I155" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J155" s="38">
+      <c r="J155" s="28">
         <v>3.0</v>
       </c>
-      <c r="K155" s="38" t="s">
+      <c r="K155" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M155" s="37" t="s">
+      <c r="L155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M155" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="N155" s="37">
+      <c r="N155" s="27">
         <v>4.0</v>
       </c>
-      <c r="O155" s="37" t="s">
+      <c r="O155" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q155" s="37" t="s">
+      <c r="P155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q155" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="R155" s="37">
+      <c r="R155" s="27">
         <v>3.0</v>
       </c>
-      <c r="S155" s="37" t="s">
+      <c r="S155" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T155" s="39"/>
-      <c r="U155" s="39"/>
-      <c r="V155" s="39"/>
-      <c r="W155" s="39"/>
-      <c r="X155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y155" s="37" t="s">
+      <c r="T155" s="21"/>
+      <c r="U155" s="21"/>
+      <c r="V155" s="21"/>
+      <c r="W155" s="21"/>
+      <c r="X155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y155" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Z155" s="37">
+      <c r="Z155" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA155" s="37" t="s">
+      <c r="AA155" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB155" s="39"/>
-      <c r="AC155" s="39"/>
-      <c r="AD155" s="39"/>
-      <c r="AE155" s="39"/>
-      <c r="AF155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG155" s="37" t="s">
+      <c r="AB155" s="21"/>
+      <c r="AC155" s="21"/>
+      <c r="AD155" s="21"/>
+      <c r="AE155" s="21"/>
+      <c r="AF155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG155" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AH155" s="37">
+      <c r="AH155" s="27">
         <v>2.0</v>
       </c>
-      <c r="AI155" s="37" t="s">
+      <c r="AI155" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="AJ155" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK155" s="37" t="s">
+      <c r="AJ155" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK155" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL155" s="37">
+      <c r="AL155" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM155" s="37" t="s">
+      <c r="AM155" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN155" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO155" s="38" t="s">
+      <c r="AN155" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO155" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AP155" s="38">
+      <c r="AP155" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ155" s="38" t="s">
+      <c r="AQ155" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR155" s="39"/>
-      <c r="AS155" s="39"/>
-      <c r="AT155" s="39"/>
-      <c r="AU155" s="39"/>
-      <c r="AV155" s="40">
+      <c r="AR155" s="21"/>
+      <c r="AS155" s="21"/>
+      <c r="AT155" s="21"/>
+      <c r="AU155" s="21"/>
+      <c r="AV155" s="30">
         <v>8.32</v>
       </c>
-      <c r="AW155" s="40">
+      <c r="AW155" s="30">
         <v>8.77</v>
       </c>
     </row>
     <row r="156" ht="18.0" customHeight="1">
-      <c r="A156" s="35">
+      <c r="A156" s="34">
         <v>154.0</v>
       </c>
-      <c r="B156" s="36" t="s">
+      <c r="B156" s="26" t="s">
         <v>438</v>
       </c>
-      <c r="C156" s="36" t="s">
+      <c r="C156" s="26" t="s">
         <v>439</v>
       </c>
-      <c r="D156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E156" s="37" t="s">
+      <c r="D156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E156" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F156" s="37">
+      <c r="F156" s="27">
         <v>4.0</v>
       </c>
-      <c r="G156" s="37" t="s">
+      <c r="G156" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I156" s="37" t="s">
+      <c r="H156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I156" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J156" s="38">
+      <c r="J156" s="28">
         <v>3.0</v>
       </c>
-      <c r="K156" s="38" t="s">
+      <c r="K156" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M156" s="37" t="s">
+      <c r="L156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M156" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="N156" s="37">
+      <c r="N156" s="27">
         <v>4.0</v>
       </c>
-      <c r="O156" s="37" t="s">
+      <c r="O156" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q156" s="37" t="s">
+      <c r="P156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q156" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="R156" s="37">
+      <c r="R156" s="27">
         <v>3.0</v>
       </c>
-      <c r="S156" s="37" t="s">
+      <c r="S156" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T156" s="39"/>
-      <c r="U156" s="39"/>
-      <c r="V156" s="39"/>
-      <c r="W156" s="39"/>
-      <c r="X156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y156" s="37" t="s">
+      <c r="T156" s="21"/>
+      <c r="U156" s="21"/>
+      <c r="V156" s="21"/>
+      <c r="W156" s="21"/>
+      <c r="X156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y156" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="Z156" s="37">
+      <c r="Z156" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA156" s="37" t="s">
+      <c r="AA156" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB156" s="39"/>
-      <c r="AC156" s="39"/>
-      <c r="AD156" s="39"/>
-      <c r="AE156" s="39"/>
-      <c r="AF156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG156" s="37" t="s">
+      <c r="AB156" s="21"/>
+      <c r="AC156" s="21"/>
+      <c r="AD156" s="21"/>
+      <c r="AE156" s="21"/>
+      <c r="AF156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG156" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AH156" s="37">
+      <c r="AH156" s="27">
         <v>2.0</v>
       </c>
-      <c r="AI156" s="37" t="s">
+      <c r="AI156" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="AJ156" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK156" s="37" t="s">
+      <c r="AJ156" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK156" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL156" s="37">
+      <c r="AL156" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM156" s="37" t="s">
+      <c r="AM156" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN156" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO156" s="38" t="s">
+      <c r="AN156" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO156" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AP156" s="38">
+      <c r="AP156" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ156" s="38" t="s">
+      <c r="AQ156" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR156" s="39"/>
-      <c r="AS156" s="39"/>
-      <c r="AT156" s="39"/>
-      <c r="AU156" s="39"/>
-      <c r="AV156" s="40">
+      <c r="AR156" s="21"/>
+      <c r="AS156" s="21"/>
+      <c r="AT156" s="21"/>
+      <c r="AU156" s="21"/>
+      <c r="AV156" s="30">
         <v>8.19</v>
       </c>
-      <c r="AW156" s="40">
+      <c r="AW156" s="30">
         <v>8.27</v>
       </c>
     </row>
     <row r="157" ht="18.0" customHeight="1">
-      <c r="A157" s="35">
+      <c r="A157" s="34">
         <v>155.0</v>
       </c>
-      <c r="B157" s="36" t="s">
+      <c r="B157" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="C157" s="36" t="s">
+      <c r="C157" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="D157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E157" s="37" t="s">
+      <c r="D157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E157" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F157" s="37">
+      <c r="F157" s="27">
         <v>4.0</v>
       </c>
-      <c r="G157" s="37" t="s">
+      <c r="G157" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I157" s="37" t="s">
+      <c r="H157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I157" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J157" s="38">
+      <c r="J157" s="28">
         <v>3.0</v>
       </c>
-      <c r="K157" s="38" t="s">
+      <c r="K157" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M157" s="37" t="s">
+      <c r="L157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M157" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N157" s="37">
+      <c r="N157" s="27">
         <v>4.0</v>
       </c>
-      <c r="O157" s="37" t="s">
+      <c r="O157" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q157" s="37" t="s">
+      <c r="P157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q157" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R157" s="37">
+      <c r="R157" s="27">
         <v>3.0</v>
       </c>
-      <c r="S157" s="37" t="s">
+      <c r="S157" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T157" s="39"/>
-      <c r="U157" s="39"/>
-      <c r="V157" s="39"/>
-      <c r="W157" s="39"/>
-      <c r="X157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y157" s="37" t="s">
+      <c r="T157" s="21"/>
+      <c r="U157" s="21"/>
+      <c r="V157" s="21"/>
+      <c r="W157" s="21"/>
+      <c r="X157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y157" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Z157" s="37">
+      <c r="Z157" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA157" s="37" t="s">
+      <c r="AA157" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB157" s="39"/>
-      <c r="AC157" s="39"/>
-      <c r="AD157" s="39"/>
-      <c r="AE157" s="39"/>
-      <c r="AF157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG157" s="37" t="s">
+      <c r="AB157" s="21"/>
+      <c r="AC157" s="21"/>
+      <c r="AD157" s="21"/>
+      <c r="AE157" s="21"/>
+      <c r="AF157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG157" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AH157" s="37">
+      <c r="AH157" s="27">
         <v>2.0</v>
       </c>
-      <c r="AI157" s="37" t="s">
+      <c r="AI157" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="AJ157" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK157" s="37" t="s">
+      <c r="AJ157" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK157" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL157" s="37">
+      <c r="AL157" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM157" s="37" t="s">
+      <c r="AM157" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN157" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO157" s="38" t="s">
+      <c r="AN157" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO157" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AP157" s="38">
+      <c r="AP157" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ157" s="38" t="s">
+      <c r="AQ157" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR157" s="39"/>
-      <c r="AS157" s="39"/>
-      <c r="AT157" s="39"/>
-      <c r="AU157" s="39"/>
-      <c r="AV157" s="40">
+      <c r="AR157" s="21"/>
+      <c r="AS157" s="21"/>
+      <c r="AT157" s="21"/>
+      <c r="AU157" s="21"/>
+      <c r="AV157" s="30">
         <v>7.37</v>
       </c>
-      <c r="AW157" s="40">
+      <c r="AW157" s="30">
         <v>7.53</v>
       </c>
     </row>
     <row r="158" ht="18.0" customHeight="1">
-      <c r="A158" s="35">
+      <c r="A158" s="34">
         <v>156.0</v>
       </c>
-      <c r="B158" s="36" t="s">
+      <c r="B158" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="C158" s="36" t="s">
+      <c r="C158" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="D158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E158" s="37" t="s">
+      <c r="D158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E158" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F158" s="37">
+      <c r="F158" s="27">
         <v>4.0</v>
       </c>
-      <c r="G158" s="37" t="s">
+      <c r="G158" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I158" s="37" t="s">
+      <c r="H158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I158" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J158" s="38">
+      <c r="J158" s="28">
         <v>3.0</v>
       </c>
-      <c r="K158" s="38" t="s">
+      <c r="K158" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M158" s="37" t="s">
+      <c r="L158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M158" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N158" s="37">
+      <c r="N158" s="27">
         <v>4.0</v>
       </c>
-      <c r="O158" s="37" t="s">
+      <c r="O158" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q158" s="37" t="s">
+      <c r="P158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q158" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="R158" s="37">
+      <c r="R158" s="27">
         <v>3.0</v>
       </c>
-      <c r="S158" s="37" t="s">
+      <c r="S158" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T158" s="39"/>
-      <c r="U158" s="39"/>
-      <c r="V158" s="39"/>
-      <c r="W158" s="39"/>
-      <c r="X158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y158" s="37" t="s">
+      <c r="T158" s="21"/>
+      <c r="U158" s="21"/>
+      <c r="V158" s="21"/>
+      <c r="W158" s="21"/>
+      <c r="X158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y158" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Z158" s="37">
+      <c r="Z158" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA158" s="37" t="s">
+      <c r="AA158" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB158" s="39"/>
-      <c r="AC158" s="39"/>
-      <c r="AD158" s="39"/>
-      <c r="AE158" s="39"/>
-      <c r="AF158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG158" s="37" t="s">
+      <c r="AB158" s="21"/>
+      <c r="AC158" s="21"/>
+      <c r="AD158" s="21"/>
+      <c r="AE158" s="21"/>
+      <c r="AF158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG158" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="AH158" s="37">
+      <c r="AH158" s="27">
         <v>2.0</v>
       </c>
-      <c r="AI158" s="37" t="s">
+      <c r="AI158" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="AJ158" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK158" s="37" t="s">
+      <c r="AJ158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK158" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL158" s="37">
+      <c r="AL158" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM158" s="37" t="s">
+      <c r="AM158" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN158" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO158" s="38" t="s">
+      <c r="AN158" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO158" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AP158" s="38">
+      <c r="AP158" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ158" s="38" t="s">
+      <c r="AQ158" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR158" s="39"/>
-      <c r="AS158" s="39"/>
-      <c r="AT158" s="39"/>
-      <c r="AU158" s="39"/>
-      <c r="AV158" s="40">
+      <c r="AR158" s="21"/>
+      <c r="AS158" s="21"/>
+      <c r="AT158" s="21"/>
+      <c r="AU158" s="21"/>
+      <c r="AV158" s="30">
         <v>7.5</v>
       </c>
-      <c r="AW158" s="40">
+      <c r="AW158" s="30">
         <v>7.34</v>
       </c>
     </row>
     <row r="159" ht="18.0" customHeight="1">
-      <c r="A159" s="35">
+      <c r="A159" s="34">
         <v>157.0</v>
       </c>
-      <c r="B159" s="36" t="s">
+      <c r="B159" s="26" t="s">
         <v>444</v>
       </c>
-      <c r="C159" s="36" t="s">
+      <c r="C159" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="D159" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E159" s="37" t="s">
+      <c r="D159" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E159" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F159" s="37">
+      <c r="F159" s="27">
         <v>4.0</v>
       </c>
-      <c r="G159" s="37" t="s">
+      <c r="G159" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H159" s="37" t="s">
+      <c r="H159" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="I159" s="37" t="s">
+      <c r="I159" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="J159" s="38">
+      <c r="J159" s="28">
         <v>0.0</v>
       </c>
-      <c r="K159" s="38" t="s">
+      <c r="K159" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L159" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M159" s="37" t="s">
+      <c r="L159" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M159" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N159" s="37">
+      <c r="N159" s="27">
         <v>4.0</v>
       </c>
-      <c r="O159" s="37" t="s">
+      <c r="O159" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="P159" s="37" t="s">
+      <c r="P159" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="Q159" s="37" t="s">
+      <c r="Q159" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="R159" s="37">
+      <c r="R159" s="27">
         <v>0.0</v>
       </c>
-      <c r="S159" s="37" t="s">
+      <c r="S159" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="T159" s="39"/>
-      <c r="U159" s="39"/>
-      <c r="V159" s="39"/>
-      <c r="W159" s="39"/>
-      <c r="X159" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y159" s="37" t="s">
+      <c r="T159" s="21"/>
+      <c r="U159" s="21"/>
+      <c r="V159" s="21"/>
+      <c r="W159" s="21"/>
+      <c r="X159" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y159" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Z159" s="37">
+      <c r="Z159" s="27">
         <v>3.0</v>
       </c>
-      <c r="AA159" s="37" t="s">
+      <c r="AA159" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AB159" s="39"/>
-      <c r="AC159" s="39"/>
-      <c r="AD159" s="39"/>
-      <c r="AE159" s="39"/>
-      <c r="AF159" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG159" s="37" t="s">
+      <c r="AB159" s="21"/>
+      <c r="AC159" s="21"/>
+      <c r="AD159" s="21"/>
+      <c r="AE159" s="21"/>
+      <c r="AF159" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG159" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AH159" s="37">
+      <c r="AH159" s="27">
         <v>2.0</v>
       </c>
-      <c r="AI159" s="37" t="s">
+      <c r="AI159" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="AJ159" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK159" s="37" t="s">
+      <c r="AJ159" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK159" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AL159" s="37">
+      <c r="AL159" s="27">
         <v>2.0</v>
       </c>
-      <c r="AM159" s="37" t="s">
+      <c r="AM159" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AN159" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO159" s="38" t="s">
+      <c r="AN159" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO159" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AP159" s="38">
+      <c r="AP159" s="28">
         <v>1.0</v>
       </c>
-      <c r="AQ159" s="38" t="s">
+      <c r="AQ159" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AR159" s="39"/>
-      <c r="AS159" s="39"/>
-      <c r="AT159" s="39"/>
-      <c r="AU159" s="39"/>
-      <c r="AV159" s="40">
+      <c r="AR159" s="21"/>
+      <c r="AS159" s="21"/>
+      <c r="AT159" s="21"/>
+      <c r="AU159" s="21"/>
+      <c r="AV159" s="30">
         <v>6.1</v>
       </c>
-      <c r="AW159" s="40">
+      <c r="AW159" s="30">
         <v>7.1</v>
       </c>
     </row>
     <row r="160" ht="18.0" customHeight="1">
-      <c r="A160" s="21"/>
-      <c r="B160" s="41"/>
-      <c r="C160" s="41"/>
-      <c r="D160" s="21"/>
-      <c r="E160" s="21"/>
-      <c r="F160" s="21"/>
-      <c r="G160" s="21"/>
-      <c r="H160" s="21"/>
-      <c r="I160" s="21"/>
-      <c r="J160" s="42"/>
-      <c r="K160" s="42"/>
-      <c r="L160" s="21"/>
-      <c r="M160" s="21"/>
-      <c r="N160" s="21"/>
-      <c r="O160" s="21"/>
-      <c r="P160" s="21"/>
-      <c r="Q160" s="21"/>
-      <c r="R160" s="21"/>
-      <c r="S160" s="21"/>
-      <c r="T160" s="21"/>
-      <c r="U160" s="21"/>
-      <c r="V160" s="21"/>
-      <c r="W160" s="21"/>
-      <c r="X160" s="21"/>
-      <c r="Y160" s="21"/>
-      <c r="Z160" s="21"/>
-      <c r="AA160" s="21"/>
-      <c r="AB160" s="21"/>
-      <c r="AC160" s="21"/>
-      <c r="AD160" s="21"/>
-      <c r="AE160" s="21"/>
-      <c r="AF160" s="21"/>
-      <c r="AG160" s="21"/>
-      <c r="AH160" s="21"/>
-      <c r="AI160" s="21"/>
-      <c r="AJ160" s="21"/>
-      <c r="AK160" s="21"/>
-      <c r="AL160" s="21"/>
-      <c r="AM160" s="21"/>
-      <c r="AN160" s="42"/>
-      <c r="AO160" s="42"/>
-      <c r="AP160" s="42"/>
-      <c r="AQ160" s="42"/>
-      <c r="AR160" s="21"/>
-      <c r="AS160" s="21"/>
-      <c r="AT160" s="21"/>
-      <c r="AU160" s="21"/>
-      <c r="AV160" s="43"/>
-      <c r="AW160" s="43"/>
+      <c r="A160" s="35">
+        <v>158.0</v>
+      </c>
+      <c r="B160" s="36" t="s">
+        <v>446</v>
+      </c>
+      <c r="C160" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="D160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E160" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F160" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="G160" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I160" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="J160" s="38">
+        <v>3.0</v>
+      </c>
+      <c r="K160" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M160" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="N160" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="O160" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P160" s="39"/>
+      <c r="Q160" s="39"/>
+      <c r="R160" s="39"/>
+      <c r="S160" s="39"/>
+      <c r="T160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="U160" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="V160" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="W160" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="X160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y160" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z160" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="AA160" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC160" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD160" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AE160" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF160" s="39"/>
+      <c r="AG160" s="39"/>
+      <c r="AH160" s="39"/>
+      <c r="AI160" s="39"/>
+      <c r="AJ160" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK160" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL160" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AM160" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN160" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO160" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP160" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="AQ160" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR160" s="39"/>
+      <c r="AS160" s="39"/>
+      <c r="AT160" s="39"/>
+      <c r="AU160" s="39"/>
+      <c r="AV160" s="40">
+        <v>8.0</v>
+      </c>
+      <c r="AW160" s="40">
+        <v>8.29</v>
+      </c>
     </row>
     <row r="161" ht="18.0" customHeight="1">
-      <c r="A161" s="44"/>
-      <c r="B161" s="41"/>
-      <c r="C161" s="41"/>
-      <c r="D161" s="21"/>
-      <c r="E161" s="21"/>
-      <c r="F161" s="21"/>
-      <c r="G161" s="21"/>
-      <c r="H161" s="21"/>
-      <c r="I161" s="21"/>
-      <c r="J161" s="42"/>
-      <c r="K161" s="42"/>
-      <c r="L161" s="21"/>
-      <c r="M161" s="21"/>
-      <c r="N161" s="21"/>
-      <c r="O161" s="21"/>
-      <c r="P161" s="21"/>
-      <c r="Q161" s="21"/>
-      <c r="R161" s="21"/>
-      <c r="S161" s="21"/>
-      <c r="T161" s="21"/>
-      <c r="U161" s="21"/>
-      <c r="V161" s="21"/>
-      <c r="W161" s="21"/>
-      <c r="X161" s="21"/>
-      <c r="Y161" s="21"/>
-      <c r="Z161" s="21"/>
-      <c r="AA161" s="21"/>
-      <c r="AB161" s="21"/>
-      <c r="AC161" s="21"/>
-      <c r="AD161" s="21"/>
-      <c r="AE161" s="21"/>
-      <c r="AF161" s="21"/>
-      <c r="AG161" s="21"/>
-      <c r="AH161" s="21"/>
-      <c r="AI161" s="21"/>
-      <c r="AJ161" s="21"/>
-      <c r="AK161" s="21"/>
-      <c r="AL161" s="21"/>
-      <c r="AM161" s="21"/>
-      <c r="AN161" s="42"/>
-      <c r="AO161" s="42"/>
-      <c r="AP161" s="42"/>
-      <c r="AQ161" s="42"/>
-      <c r="AR161" s="21"/>
-      <c r="AS161" s="21"/>
-      <c r="AT161" s="21"/>
-      <c r="AU161" s="21"/>
-      <c r="AV161" s="43"/>
-      <c r="AW161" s="43"/>
+      <c r="A161" s="35">
+        <v>159.0</v>
+      </c>
+      <c r="B161" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="C161" s="36" t="s">
+        <v>449</v>
+      </c>
+      <c r="D161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F161" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="G161" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I161" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J161" s="38">
+        <v>3.0</v>
+      </c>
+      <c r="K161" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M161" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="N161" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="O161" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P161" s="39"/>
+      <c r="Q161" s="39"/>
+      <c r="R161" s="39"/>
+      <c r="S161" s="39"/>
+      <c r="T161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="U161" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="V161" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="W161" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="X161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y161" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z161" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="AA161" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC161" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD161" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AE161" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF161" s="39"/>
+      <c r="AG161" s="39"/>
+      <c r="AH161" s="39"/>
+      <c r="AI161" s="39"/>
+      <c r="AJ161" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK161" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL161" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AM161" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN161" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO161" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP161" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="AQ161" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR161" s="39"/>
+      <c r="AS161" s="39"/>
+      <c r="AT161" s="39"/>
+      <c r="AU161" s="39"/>
+      <c r="AV161" s="40">
+        <v>8.28</v>
+      </c>
+      <c r="AW161" s="40">
+        <v>8.7</v>
+      </c>
     </row>
     <row r="162" ht="18.0" customHeight="1">
-      <c r="A162" s="21"/>
-      <c r="B162" s="41"/>
-      <c r="C162" s="41"/>
-      <c r="D162" s="21"/>
-      <c r="E162" s="21"/>
-      <c r="F162" s="21"/>
-      <c r="G162" s="21"/>
-      <c r="H162" s="21"/>
-      <c r="I162" s="21"/>
-      <c r="J162" s="42"/>
-      <c r="K162" s="42"/>
-      <c r="L162" s="21"/>
-      <c r="M162" s="21"/>
-      <c r="N162" s="21"/>
-      <c r="O162" s="21"/>
-      <c r="P162" s="21"/>
-      <c r="Q162" s="21"/>
-      <c r="R162" s="21"/>
-      <c r="S162" s="21"/>
-      <c r="T162" s="21"/>
-      <c r="U162" s="21"/>
-      <c r="V162" s="21"/>
-      <c r="W162" s="21"/>
-      <c r="X162" s="21"/>
-      <c r="Y162" s="21"/>
-      <c r="Z162" s="21"/>
-      <c r="AA162" s="21"/>
-      <c r="AB162" s="21"/>
-      <c r="AC162" s="21"/>
-      <c r="AD162" s="21"/>
-      <c r="AE162" s="21"/>
-      <c r="AF162" s="21"/>
-      <c r="AG162" s="21"/>
-      <c r="AH162" s="21"/>
-      <c r="AI162" s="21"/>
-      <c r="AJ162" s="21"/>
-      <c r="AK162" s="21"/>
-      <c r="AL162" s="21"/>
-      <c r="AM162" s="21"/>
-      <c r="AN162" s="42"/>
-      <c r="AO162" s="42"/>
-      <c r="AP162" s="42"/>
-      <c r="AQ162" s="42"/>
-      <c r="AR162" s="21"/>
-      <c r="AS162" s="21"/>
-      <c r="AT162" s="21"/>
-      <c r="AU162" s="21"/>
-      <c r="AV162" s="43"/>
-      <c r="AW162" s="43"/>
+      <c r="A162" s="35">
+        <v>160.0</v>
+      </c>
+      <c r="B162" s="36" t="s">
+        <v>450</v>
+      </c>
+      <c r="C162" s="36" t="s">
+        <v>451</v>
+      </c>
+      <c r="D162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F162" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="G162" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I162" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J162" s="38">
+        <v>3.0</v>
+      </c>
+      <c r="K162" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M162" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="N162" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="O162" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q162" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="R162" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="S162" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="T162" s="39"/>
+      <c r="U162" s="39"/>
+      <c r="V162" s="39"/>
+      <c r="W162" s="39"/>
+      <c r="X162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y162" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z162" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="AA162" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB162" s="39"/>
+      <c r="AC162" s="39"/>
+      <c r="AD162" s="39"/>
+      <c r="AE162" s="39"/>
+      <c r="AF162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG162" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH162" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AI162" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ162" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK162" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL162" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AM162" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN162" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO162" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP162" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="AQ162" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR162" s="39"/>
+      <c r="AS162" s="39"/>
+      <c r="AT162" s="39"/>
+      <c r="AU162" s="39"/>
+      <c r="AV162" s="40">
+        <v>8.96</v>
+      </c>
+      <c r="AW162" s="40">
+        <v>9.34</v>
+      </c>
     </row>
     <row r="163" ht="18.0" customHeight="1">
-      <c r="A163" s="44"/>
-      <c r="B163" s="41"/>
-      <c r="C163" s="41"/>
-      <c r="D163" s="21"/>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="21"/>
-      <c r="H163" s="21"/>
-      <c r="I163" s="21"/>
-      <c r="J163" s="42"/>
-      <c r="K163" s="42"/>
-      <c r="L163" s="21"/>
-      <c r="M163" s="21"/>
-      <c r="N163" s="21"/>
-      <c r="O163" s="21"/>
-      <c r="P163" s="21"/>
-      <c r="Q163" s="21"/>
-      <c r="R163" s="21"/>
-      <c r="S163" s="21"/>
-      <c r="T163" s="21"/>
-      <c r="U163" s="21"/>
-      <c r="V163" s="21"/>
-      <c r="W163" s="21"/>
-      <c r="X163" s="21"/>
-      <c r="Y163" s="21"/>
-      <c r="Z163" s="21"/>
-      <c r="AA163" s="21"/>
-      <c r="AB163" s="21"/>
-      <c r="AC163" s="21"/>
-      <c r="AD163" s="21"/>
-      <c r="AE163" s="21"/>
-      <c r="AF163" s="21"/>
-      <c r="AG163" s="21"/>
-      <c r="AH163" s="21"/>
-      <c r="AI163" s="21"/>
-      <c r="AJ163" s="21"/>
-      <c r="AK163" s="21"/>
-      <c r="AL163" s="21"/>
-      <c r="AM163" s="21"/>
-      <c r="AN163" s="42"/>
-      <c r="AO163" s="42"/>
-      <c r="AP163" s="42"/>
-      <c r="AQ163" s="42"/>
-      <c r="AR163" s="21"/>
-      <c r="AS163" s="21"/>
-      <c r="AT163" s="21"/>
-      <c r="AU163" s="21"/>
-      <c r="AV163" s="43"/>
-      <c r="AW163" s="43"/>
+      <c r="A163" s="35">
+        <v>161.0</v>
+      </c>
+      <c r="B163" s="36" t="s">
+        <v>452</v>
+      </c>
+      <c r="C163" s="36" t="s">
+        <v>453</v>
+      </c>
+      <c r="D163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E163" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F163" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="G163" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I163" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J163" s="38">
+        <v>3.0</v>
+      </c>
+      <c r="K163" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="M163" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="N163" s="37">
+        <v>4.0</v>
+      </c>
+      <c r="O163" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="P163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q163" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="R163" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="S163" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="T163" s="39"/>
+      <c r="U163" s="39"/>
+      <c r="V163" s="39"/>
+      <c r="W163" s="39"/>
+      <c r="X163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y163" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z163" s="37">
+        <v>3.0</v>
+      </c>
+      <c r="AA163" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB163" s="39"/>
+      <c r="AC163" s="39"/>
+      <c r="AD163" s="39"/>
+      <c r="AE163" s="39"/>
+      <c r="AF163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG163" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH163" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AI163" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ163" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK163" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL163" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="AM163" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN163" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO163" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AP163" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="AQ163" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR163" s="39"/>
+      <c r="AS163" s="39"/>
+      <c r="AT163" s="39"/>
+      <c r="AU163" s="39"/>
+      <c r="AV163" s="40">
+        <v>8.78</v>
+      </c>
+      <c r="AW163" s="40">
+        <v>9.29</v>
+      </c>
     </row>
     <row r="164" ht="18.0" customHeight="1">
       <c r="A164" s="21"/>

</xml_diff>